<commit_message>
Added feature to store Output Data in Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/data.xlsx
+++ b/src/test/resources/excel/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303561\eclipse-workspace\Flipkart\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100632C4-D179-4710-B91B-43A26E29118E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ADD492-F559-4E69-8003-56037F8EE670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestInputData" sheetId="1" r:id="rId1"/>
+    <sheet name="TestOutputData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,18 +26,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Browser Name</t>
   </si>
   <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>Product Name</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>Samsung galaxy s24 ultra</t>
+    <t>Samsung Galaxy S24 Ultra</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy S24 Ultra 5G (Titanium Violet, 256 GB)</t>
+  </si>
+  <si>
+    <t>₹1,29,999</t>
   </si>
 </sst>
 </file>
@@ -356,14 +366,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -371,15 +381,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ScreenShot feature and did minor fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/data.xlsx
+++ b/src/test/resources/excel/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303561\eclipse-workspace\Flipkart\src\test\resources\excel\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Browser Name</t>
   </si>
@@ -53,6 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,8 +373,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.19921875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -405,11 +406,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="48.8984375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.8984375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -417,7 +418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added Screen Shots in ExtentReports
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/data.xlsx
+++ b/src/test/resources/excel/data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="8">
   <si>
     <t>Browser Name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>₹1,29,999</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy S24 Ultra 5G (Titanium Black, 256 GB)</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added multi browser testing feature based on excel input data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/data.xlsx
+++ b/src/test/resources/excel/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303561\eclipse-workspace\Flipkart\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303561\eclipse-workspace\Flipkart-S24\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD7CD16-5FBC-4868-A328-1AECA60D3C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2E9A0-C3B9-490A-830C-479ABCA61137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestInputData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
   <si>
     <t>Chrome</t>
   </si>
@@ -46,9 +46,6 @@
     <t>₹1,29,999</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -80,6 +77,12 @@
   </si>
   <si>
     <t>₹1,09,999</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -398,32 +401,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.796875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.19921875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.796875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.21875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -438,10 +447,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="48.8984375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.8984375"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="48.88671875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.88671875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -454,7 +463,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -462,7 +471,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -478,42 +487,42 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Headless browser mode and Parallel browser testing
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/data.xlsx
+++ b/src/test/resources/excel/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303561\eclipse-workspace\Flipkart-S24\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2E9A0-C3B9-490A-830C-479ABCA61137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B8BA05-3DD5-4384-8A7D-30EE80CCA0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
   <si>
     <t>Chrome</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>₹1,59,999</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy S22 ultra 5G (Burgundy, 256 GB)</t>
-  </si>
-  <si>
-    <t>₹1,09,999</t>
   </si>
   <si>
     <t>Edge</t>
@@ -404,7 +398,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,7 +413,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -427,10 +421,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -443,9 +437,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -471,7 +467,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -479,7 +475,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -515,14 +511,6 @@
       </c>
       <c r="B8" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>